<commit_message>
Update Mitigation implementations timelines.xlsx
</commit_message>
<xml_diff>
--- a/Data Archive/Mitigation implementations timelines.xlsx
+++ b/Data Archive/Mitigation implementations timelines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/GitHub/CovidPolicy-Canada/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30E2B55-63B6-5942-8303-0DDE1CD1BDE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A792FC1-98D2-B341-86E0-3860F8093EB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alberta" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="1242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="1260">
   <si>
     <t>03/30/2020</t>
   </si>
@@ -11007,6 +11007,62 @@
   </si>
   <si>
     <t>Spring breat (https://www.cbe.ab.ca/registration/calendars/Documents/2021-2022-Modified-Calendar.pdf)</t>
+  </si>
+  <si>
+    <t>06/14/2022</t>
+  </si>
+  <si>
+    <t>All mandatory public health restrictions were lifted on June 14 as the Omicron BA.2 wave subsides and COVID-19 hospitalizations continues to decline.(https://www.alberta.ca/covid-19-public-health-actions.aspx)</t>
+  </si>
+  <si>
+    <t>06/11/2022</t>
+  </si>
+  <si>
+    <t>Remaining masking requirements removed. (https://news.ontario.ca/en/statement/1002160/most-masking-requirements-to-be-lifted-on-june-11)</t>
+  </si>
+  <si>
+    <t>2/28/2022</t>
+  </si>
+  <si>
+    <t>As of February 28 2022, non-medical masks will continue to be required when traveling on Saskatoon Transit vehicles. This applies to all customers, including those who have been vaccinated.(https://transit.saskatoon.ca/rider-guide/covid-19/face-masks#:~:text=As%20of%20February%2028%202022,those%20who%20have%20been%20vaccinated.)</t>
+  </si>
+  <si>
+    <t>06/28/2022</t>
+  </si>
+  <si>
+    <t>Mandatory masking lifted in public transit. (https://saskatoon.ctvnews.ca/saskatoon-transit-to-end-covid-19-mask-requirement-1.5966782)</t>
+  </si>
+  <si>
+    <t>06/18/2022</t>
+  </si>
+  <si>
+    <t>Mandatory masking in public transit is lifted. Masks still mandatory in hospitals, long-term care homes, other health-care facilities. (https://www.cbc.ca/news/canada/montreal/end-of-masking-on-public-transit-1.6493553)</t>
+  </si>
+  <si>
+    <t>07/04/2022</t>
+  </si>
+  <si>
+    <t>Masks are no longer mandatory for health facilities across Nunavut. Masks are also no longer mandatory in Nunavut schools and government workplaces. (https://www.thesafetymag.com/ca/topics/occupational-hygiene/nunavut-lifts-mask-mandate-in-health-facilities-workplaces/412176)</t>
+  </si>
+  <si>
+    <t>07/14/2022</t>
+  </si>
+  <si>
+    <t>Vaccination no longer required for workers, volunteers and contractors working in high-risk settings. Some settings may require you to wear a mask such as in long-term care homes, health facilities, shelters, group homes, the correctional centre and hospitals. (https://yukon.ca/en/news/update-covid-19-yukon). As of july 14. 2022, residents are still required to wear a mask in places such as:
+schools; long-term care homes; health facilities; shelters; group homes; the correctional centre; and hospitals.(xhttps://yukon.ca/en/health-and-wellness/covid-19-information/your-health-covid-19/wearing-non-medical-mask-yukon)</t>
+  </si>
+  <si>
+    <t>07/06/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All remaining Covid-19 restrictions are dropped. Indoor masking will shift to “optional” from strongly recommended unless somebody is ill or the indoor setting is crowded. And people who get the virus will no longer be required to isolate, although it will still be strongly recommended.(https://www.thesafetymag.com/ca/topics/occupational-hygiene/nunavut-lifts-mask-mandate-in-health-facilities-workplaces/412176)
+</t>
+  </si>
+  <si>
+    <t>06/03/2022</t>
+  </si>
+  <si>
+    <t>As of June 3, 2022, masks are still recommended but not longer required in public transit.(https://www.princeedwardisland.ca/en/information/health-and-wellness/wearing-masks-in-the-community-and-workplaces)</t>
   </si>
 </sst>
 </file>
@@ -11230,7 +11286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -11635,6 +11691,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -11653,6 +11716,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11973,9 +12039,9 @@
   </sheetPr>
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
+    <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -12374,7 +12440,13 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="49" spans="3:3" ht="51">
+    <row r="49" spans="1:3" ht="51">
+      <c r="A49" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B49" s="88" t="s">
+        <v>1243</v>
+      </c>
       <c r="C49" s="102" t="s">
         <v>617</v>
       </c>
@@ -12389,10 +12461,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" zoomScale="107" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView topLeftCell="A66" zoomScale="107" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -12721,16 +12793,16 @@
       </c>
     </row>
     <row r="40" spans="1:2" s="71" customFormat="1" ht="226" customHeight="1">
-      <c r="A40" s="182" t="s">
+      <c r="A40" s="185" t="s">
         <v>813</v>
       </c>
-      <c r="B40" s="184" t="s">
+      <c r="B40" s="187" t="s">
         <v>814</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="71" customFormat="1" ht="232" customHeight="1">
-      <c r="A41" s="183"/>
-      <c r="B41" s="184"/>
+      <c r="A41" s="186"/>
+      <c r="B41" s="187"/>
     </row>
     <row r="42" spans="1:2" ht="34">
       <c r="A42" s="70" t="s">
@@ -12741,28 +12813,28 @@
       </c>
     </row>
     <row r="43" spans="1:2" s="71" customFormat="1" ht="324" customHeight="1">
-      <c r="A43" s="182" t="s">
+      <c r="A43" s="185" t="s">
         <v>121</v>
       </c>
-      <c r="B43" s="184" t="s">
+      <c r="B43" s="187" t="s">
         <v>819</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="71" customFormat="1" ht="134" customHeight="1">
-      <c r="A44" s="183"/>
-      <c r="B44" s="184"/>
+      <c r="A44" s="186"/>
+      <c r="B44" s="187"/>
     </row>
     <row r="45" spans="1:2" s="71" customFormat="1" ht="186" customHeight="1">
-      <c r="A45" s="180" t="s">
+      <c r="A45" s="183" t="s">
         <v>448</v>
       </c>
-      <c r="B45" s="184" t="s">
+      <c r="B45" s="187" t="s">
         <v>820</v>
       </c>
     </row>
     <row r="46" spans="1:2" s="71" customFormat="1" ht="284" customHeight="1">
-      <c r="A46" s="185"/>
-      <c r="B46" s="184"/>
+      <c r="A46" s="188"/>
+      <c r="B46" s="187"/>
     </row>
     <row r="47" spans="1:2" ht="17">
       <c r="A47" s="70" t="s">
@@ -12789,28 +12861,28 @@
       </c>
     </row>
     <row r="50" spans="1:2" s="71" customFormat="1" ht="212" customHeight="1">
-      <c r="A50" s="182" t="s">
+      <c r="A50" s="185" t="s">
         <v>824</v>
       </c>
-      <c r="B50" s="184" t="s">
+      <c r="B50" s="187" t="s">
         <v>940</v>
       </c>
     </row>
     <row r="51" spans="1:2" s="71" customFormat="1" ht="224" customHeight="1">
-      <c r="A51" s="183"/>
-      <c r="B51" s="184"/>
+      <c r="A51" s="186"/>
+      <c r="B51" s="187"/>
     </row>
     <row r="52" spans="1:2" s="71" customFormat="1" ht="232" customHeight="1">
-      <c r="A52" s="182" t="s">
+      <c r="A52" s="185" t="s">
         <v>825</v>
       </c>
-      <c r="B52" s="184" t="s">
+      <c r="B52" s="187" t="s">
         <v>939</v>
       </c>
     </row>
     <row r="53" spans="1:2" s="71" customFormat="1" ht="242" customHeight="1">
-      <c r="A53" s="183"/>
-      <c r="B53" s="184"/>
+      <c r="A53" s="186"/>
+      <c r="B53" s="187"/>
     </row>
     <row r="54" spans="1:2" ht="34">
       <c r="A54" s="70" t="s">
@@ -12938,6 +13010,14 @@
       </c>
       <c r="B69" s="169" t="s">
         <v>1227</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="51">
+      <c r="A70" s="1" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B70" s="181" t="s">
+        <v>1257</v>
       </c>
     </row>
   </sheetData>
@@ -12964,7 +13044,7 @@
   </sheetPr>
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
@@ -13409,7 +13489,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -13735,10 +13815,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -14029,6 +14109,14 @@
       </c>
       <c r="B35" s="169" t="s">
         <v>1230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="34">
+      <c r="A36" s="1" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B36" s="181" t="s">
+        <v>1259</v>
       </c>
     </row>
   </sheetData>
@@ -14172,24 +14260,24 @@
       </c>
     </row>
     <row r="14" spans="1:15" s="64" customFormat="1" ht="81" customHeight="1">
-      <c r="A14" s="186" t="s">
+      <c r="A14" s="189" t="s">
         <v>255</v>
       </c>
-      <c r="B14" s="184" t="s">
+      <c r="B14" s="187" t="s">
         <v>727</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="64" customFormat="1" ht="71" customHeight="1">
-      <c r="A15" s="187"/>
-      <c r="B15" s="184"/>
+      <c r="A15" s="190"/>
+      <c r="B15" s="187"/>
     </row>
     <row r="16" spans="1:15" s="64" customFormat="1" ht="95" customHeight="1">
-      <c r="A16" s="187"/>
-      <c r="B16" s="184"/>
+      <c r="A16" s="190"/>
+      <c r="B16" s="187"/>
     </row>
     <row r="17" spans="1:2" s="64" customFormat="1" ht="192" customHeight="1">
-      <c r="A17" s="187"/>
-      <c r="B17" s="184"/>
+      <c r="A17" s="190"/>
+      <c r="B17" s="187"/>
     </row>
     <row r="18" spans="1:2" s="64" customFormat="1" ht="192" customHeight="1">
       <c r="A18" s="69" t="s">
@@ -14687,8 +14775,8 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView zoomScale="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -15197,11 +15285,11 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -15694,6 +15782,14 @@
         <v>1175</v>
       </c>
     </row>
+    <row r="59" spans="1:2" ht="17">
+      <c r="A59" s="6" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B59" s="181" t="s">
+        <v>1245</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C40" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15705,11 +15801,11 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -16060,20 +16156,37 @@
       </c>
       <c r="C41" s="175"/>
     </row>
-    <row r="42" spans="1:3" ht="41" customHeight="1">
+    <row r="42" spans="1:3" s="180" customFormat="1" ht="51">
       <c r="A42" s="6" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C42" s="181"/>
+    </row>
+    <row r="43" spans="1:3" ht="41" customHeight="1">
+      <c r="A43" s="6" t="s">
         <v>1170</v>
       </c>
-      <c r="B42" s="46" t="s">
+      <c r="B43" s="46" t="s">
         <v>1232</v>
       </c>
-      <c r="C42" s="90" t="s">
+      <c r="C43" s="90" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17">
+      <c r="A44" s="6" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B44" s="191" t="s">
+        <v>1249</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B42" r:id="rId1" display="https://globalnews.ca/tag/saskatchewan-schools/" xr:uid="{8E8EA5DC-B0DA-0741-95A7-6437D0DA5D1F}"/>
+    <hyperlink ref="B43" r:id="rId1" display="https://globalnews.ca/tag/saskatchewan-schools/" xr:uid="{8E8EA5DC-B0DA-0741-95A7-6437D0DA5D1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16084,11 +16197,11 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C124"/>
+  <dimension ref="A1:C125"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B125" sqref="B125"/>
+      <selection pane="bottomLeft" activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -17143,6 +17256,14 @@
       </c>
       <c r="B124" s="167" t="s">
         <v>1218</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="34">
+      <c r="A125" s="6" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B125" s="181" t="s">
+        <v>1251</v>
       </c>
     </row>
   </sheetData>
@@ -17164,7 +17285,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -17555,10 +17676,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -17843,20 +17964,20 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="408" customHeight="1">
-      <c r="A34" s="180" t="s">
+      <c r="A34" s="183" t="s">
         <v>269</v>
       </c>
-      <c r="B34" s="179" t="s">
+      <c r="B34" s="182" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="206" customHeight="1">
-      <c r="A35" s="180"/>
-      <c r="B35" s="179"/>
+      <c r="A35" s="183"/>
+      <c r="B35" s="182"/>
     </row>
     <row r="36" spans="1:3" s="43" customFormat="1" ht="138" customHeight="1">
-      <c r="A36" s="181"/>
-      <c r="B36" s="179"/>
+      <c r="A36" s="184"/>
+      <c r="B36" s="182"/>
     </row>
     <row r="37" spans="1:3" s="43" customFormat="1" ht="51">
       <c r="A37" s="1" t="s">
@@ -17973,16 +18094,16 @@
       </c>
     </row>
     <row r="50" spans="1:2" s="86" customFormat="1" ht="229" customHeight="1">
-      <c r="A50" s="182" t="s">
+      <c r="A50" s="185" t="s">
         <v>903</v>
       </c>
-      <c r="B50" s="179" t="s">
+      <c r="B50" s="182" t="s">
         <v>904</v>
       </c>
     </row>
     <row r="51" spans="1:2" s="86" customFormat="1" ht="181" customHeight="1">
-      <c r="A51" s="183"/>
-      <c r="B51" s="179"/>
+      <c r="A51" s="186"/>
+      <c r="B51" s="182"/>
     </row>
     <row r="52" spans="1:2" ht="17">
       <c r="A52" s="103" t="s">
@@ -18078,6 +18199,14 @@
       </c>
       <c r="B63" s="168" t="s">
         <v>1219</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="34">
+      <c r="A64" s="103" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B64" s="179" t="s">
+        <v>1253</v>
       </c>
     </row>
   </sheetData>
@@ -18098,9 +18227,9 @@
   </sheetPr>
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -18799,10 +18928,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -19094,6 +19223,14 @@
         <v>1237</v>
       </c>
     </row>
+    <row r="36" spans="1:2" ht="119">
+      <c r="A36" s="1" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B36" s="181" t="s">
+        <v>1255</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>